<commit_message>
added real estate and changed some icons
</commit_message>
<xml_diff>
--- a/CamerHire.xlsx
+++ b/CamerHire.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjeut\Documents\Businesses\CamerHire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E753CF6-C9CF-4748-9BCB-9260865D4F13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8C07AC-FD82-4FD8-9690-39673890063D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{8FC2D6FF-FB2F-429B-AC52-C7EE5688EC2B}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{8FC2D6FF-FB2F-429B-AC52-C7EE5688EC2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Entertainment" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="Youtube" sheetId="3" r:id="rId3"/>
     <sheet name="Online" sheetId="4" r:id="rId4"/>
     <sheet name="All Auto" sheetId="7" r:id="rId5"/>
-    <sheet name="Other" sheetId="6" r:id="rId6"/>
+    <sheet name="Real Est Agent" sheetId="8" r:id="rId6"/>
+    <sheet name="Other" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="131">
   <si>
     <t>Company</t>
   </si>
@@ -395,6 +396,42 @@
   </si>
   <si>
     <t>828-559-2110</t>
+  </si>
+  <si>
+    <t>Agent</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>Claire Mafouomene</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>202-369-2720</t>
+  </si>
+  <si>
+    <t>Maryland</t>
+  </si>
+  <si>
+    <t>www.investplusrealestate.com</t>
+  </si>
+  <si>
+    <t>Marie-Noelle Metseye</t>
+  </si>
+  <si>
+    <t>410-300-3164</t>
+  </si>
+  <si>
+    <t>cmafouomene@gmail.com</t>
+  </si>
+  <si>
+    <t>mmetseye@gmail.com</t>
+  </si>
+  <si>
+    <t>www.mnlrealestate.com</t>
   </si>
 </sst>
 </file>
@@ -449,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -491,6 +528,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1426,8 +1466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE207F6-15B4-40A0-8E50-1BE50B7C015A}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1602,6 +1642,91 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCF034A5-6804-4E5E-9255-0E833B3465BB}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="4" max="4" width="29.88671875" customWidth="1"/>
+    <col min="5" max="5" width="35.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="9" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="9" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="9" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:5" s="9" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:5" s="9" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:5" s="9" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:5" s="9" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:5" s="9" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:5" s="9" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{26DD4AA5-26D3-4209-9D0A-62552AEF7287}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{06A72DE8-BB76-4FBE-A7E1-3E994A4A5BF4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CBE6F7A-AD57-4A5C-9CED-95D0DEAC1C87}">
   <dimension ref="A1:I18"/>
   <sheetViews>

</xml_diff>

<commit_message>
added more contact and more items
</commit_message>
<xml_diff>
--- a/CamerHire.xlsx
+++ b/CamerHire.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjeut\Documents\Businesses\CamerHire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8C07AC-FD82-4FD8-9690-39673890063D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C0ECA5-B9B2-49F9-90F6-F229ED99DE4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{8FC2D6FF-FB2F-429B-AC52-C7EE5688EC2B}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8FC2D6FF-FB2F-429B-AC52-C7EE5688EC2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Entertainment" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="135">
   <si>
     <t>Company</t>
   </si>
@@ -432,6 +432,18 @@
   </si>
   <si>
     <t>www.mnlrealestate.com</t>
+  </si>
+  <si>
+    <t>Udemy</t>
+  </si>
+  <si>
+    <t>If you want to remain competive today and tomorrow, you will have to learn how to code. The way data is beeing aggresively collected by almost every industries is the proof that those can code or analyze data will be trivial. For example during the covid, a lot of people lost their jobs, but the ones that will integrate new jobs faster are those who can code or analyze data. I encourage you to take this course I prepared and posted on Udemy. It's an introduction to the R programming language with a modern touch to it. Use the coupon code LEARNR to get it for $12.99.</t>
+  </si>
+  <si>
+    <t>Robert Jeutong</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/introduction-to-programming-r-a-modern-approach</t>
   </si>
 </sst>
 </file>
@@ -972,19 +984,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AD356C-CD42-4914-9103-018D0AD79E33}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.5546875" customWidth="1"/>
-    <col min="2" max="2" width="67.6640625" customWidth="1"/>
+    <col min="2" max="2" width="77.21875" customWidth="1"/>
     <col min="3" max="3" width="14.77734375" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="21.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" customWidth="1"/>
+    <col min="5" max="5" width="38.6640625" customWidth="1"/>
     <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1023,6 +1035,24 @@
         <v>45</v>
       </c>
       <c r="F2" s="11"/>
+    </row>
+    <row r="3" spans="1:6" s="3" customFormat="1" ht="143.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="F3" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1645,7 +1675,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCF034A5-6804-4E5E-9255-0E833B3465BB}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
More items. Added containers
</commit_message>
<xml_diff>
--- a/CamerHire.xlsx
+++ b/CamerHire.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjeut\Documents\Businesses\CamerHire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C0ECA5-B9B2-49F9-90F6-F229ED99DE4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFFE42F-DED8-4556-9B9A-17A925ED6A3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8FC2D6FF-FB2F-429B-AC52-C7EE5688EC2B}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{8FC2D6FF-FB2F-429B-AC52-C7EE5688EC2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Entertainment" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="Online" sheetId="4" r:id="rId4"/>
     <sheet name="All Auto" sheetId="7" r:id="rId5"/>
     <sheet name="Real Est Agent" sheetId="8" r:id="rId6"/>
-    <sheet name="Other" sheetId="6" r:id="rId7"/>
+    <sheet name="Conteners" sheetId="9" r:id="rId7"/>
+    <sheet name="Other" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="144">
   <si>
     <t>Company</t>
   </si>
@@ -444,6 +445,33 @@
   </si>
   <si>
     <t>https://www.udemy.com/course/introduction-to-programming-r-a-modern-approach</t>
+  </si>
+  <si>
+    <t>Web</t>
+  </si>
+  <si>
+    <t>www.Etgcm.com</t>
+  </si>
+  <si>
+    <t>Papy Dollars Chonelaz</t>
+  </si>
+  <si>
+    <t>14388797423 / 14385303016 / 237676457392</t>
+  </si>
+  <si>
+    <t>CANADA</t>
+  </si>
+  <si>
+    <t>Chargement de conteners du Canada pour Douala (Trois Rivière, Québec, Ottawa, Gatineau et Torronto). Appel, text ou whatsApp. Visiter leur site pour les photos et plus d'info.</t>
+  </si>
+  <si>
+    <t>Pour toutes vos annonces de recherche ou de location d’espace dans un conteneur en direction du Cameroun en particulier et de l’Afrique en général, ce groupe vous permet de diffuser vos annonces</t>
+  </si>
+  <si>
+    <t>Yannick KG</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/groups/261597531737645/?ref=share</t>
   </si>
 </sst>
 </file>
@@ -498,7 +526,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -543,6 +571,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -986,7 +1017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8AD356C-CD42-4914-9103-018D0AD79E33}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -1676,7 +1707,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1757,6 +1788,78 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F10B21B-5C1E-4E58-B7B1-B16C998DB521}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="32.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="47.5546875" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="9" customFormat="1" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="9" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CBE6F7A-AD57-4A5C-9CED-95D0DEAC1C87}">
   <dimension ref="A1:I18"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added Toussaint and Gisele. Plus Food category.
</commit_message>
<xml_diff>
--- a/CamerHire.xlsx
+++ b/CamerHire.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjeut\Documents\Businesses\CamerHire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFFE42F-DED8-4556-9B9A-17A925ED6A3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C0E09D-89B2-4E39-9DF2-368464616D40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{8FC2D6FF-FB2F-429B-AC52-C7EE5688EC2B}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{8FC2D6FF-FB2F-429B-AC52-C7EE5688EC2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Entertainment" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,8 @@
     <sheet name="All Auto" sheetId="7" r:id="rId5"/>
     <sheet name="Real Est Agent" sheetId="8" r:id="rId6"/>
     <sheet name="Conteners" sheetId="9" r:id="rId7"/>
-    <sheet name="Other" sheetId="6" r:id="rId8"/>
+    <sheet name="Food" sheetId="10" r:id="rId8"/>
+    <sheet name="Other" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="156">
   <si>
     <t>Company</t>
   </si>
@@ -472,6 +473,42 @@
   </si>
   <si>
     <t>https://www.facebook.com/groups/261597531737645/?ref=share</t>
+  </si>
+  <si>
+    <t>Contact Name</t>
+  </si>
+  <si>
+    <t>Loveline Waino</t>
+  </si>
+  <si>
+    <t>Hello friends, we cater for all events 😊give us a call</t>
+  </si>
+  <si>
+    <t>240-898-7306, 240-821-0400</t>
+  </si>
+  <si>
+    <t>silver Spring MD, DC, VA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/channel/UCl4sddVsOpiNT3bh2aDHoFg</t>
+  </si>
+  <si>
+    <t>Un Prince Dans la Plantation</t>
+  </si>
+  <si>
+    <t>Faits divers</t>
+  </si>
+  <si>
+    <t>Toussaint Louverture</t>
+  </si>
+  <si>
+    <t>Gigi's Loc Garden</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/channel/UCoLcRPx4nWLKOKQQU4Lz1_A</t>
+  </si>
+  <si>
+    <t>Gisele Exquise</t>
   </si>
 </sst>
 </file>
@@ -1094,15 +1131,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68374359-F7EA-4905-9E48-1A756A97AD72}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
     <col min="2" max="2" width="55.88671875" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1"/>
     <col min="4" max="4" width="73.33203125" customWidth="1"/>
     <col min="5" max="5" width="53.44140625" customWidth="1"/>
   </cols>
@@ -1206,18 +1243,34 @@
       <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" s="3" customFormat="1" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="13"/>
+      <c r="A7" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>149</v>
+      </c>
       <c r="E7" s="9"/>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="1:6" s="3" customFormat="1" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="13"/>
+    <row r="8" spans="1:6" s="3" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>154</v>
+      </c>
       <c r="E8" s="9"/>
       <c r="F8" s="11"/>
     </row>
@@ -1791,7 +1844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F10B21B-5C1E-4E58-B7B1-B16C998DB521}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1860,11 +1913,137 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D0572C1-3AB9-4C43-A304-72BCFF440683}">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+    </row>
+    <row r="2" spans="1:9" s="3" customFormat="1" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" spans="1:9" s="3" customFormat="1" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="11"/>
+    </row>
+    <row r="4" spans="1:9" s="3" customFormat="1" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="11"/>
+    </row>
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="11"/>
+    </row>
+    <row r="6" spans="1:9" s="3" customFormat="1" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="11"/>
+    </row>
+    <row r="7" spans="1:9" s="3" customFormat="1" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="11"/>
+    </row>
+    <row r="8" spans="1:9" s="3" customFormat="1" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CBE6F7A-AD57-4A5C-9CED-95D0DEAC1C87}">
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added hair category, plus a few more items
</commit_message>
<xml_diff>
--- a/CamerHire.xlsx
+++ b/CamerHire.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjeut\Documents\Businesses\CamerHire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C0E09D-89B2-4E39-9DF2-368464616D40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983FD54F-072A-4485-802E-563A38635E9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{8FC2D6FF-FB2F-429B-AC52-C7EE5688EC2B}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{8FC2D6FF-FB2F-429B-AC52-C7EE5688EC2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Entertainment" sheetId="1" r:id="rId1"/>
     <sheet name="Education" sheetId="2" r:id="rId2"/>
     <sheet name="Youtube" sheetId="3" r:id="rId3"/>
     <sheet name="Online" sheetId="4" r:id="rId4"/>
-    <sheet name="All Auto" sheetId="7" r:id="rId5"/>
-    <sheet name="Real Est Agent" sheetId="8" r:id="rId6"/>
-    <sheet name="Conteners" sheetId="9" r:id="rId7"/>
-    <sheet name="Food" sheetId="10" r:id="rId8"/>
-    <sheet name="Other" sheetId="6" r:id="rId9"/>
+    <sheet name="Hair" sheetId="11" r:id="rId5"/>
+    <sheet name="All Auto" sheetId="7" r:id="rId6"/>
+    <sheet name="Real Est Agent" sheetId="8" r:id="rId7"/>
+    <sheet name="Conteners" sheetId="9" r:id="rId8"/>
+    <sheet name="Food" sheetId="10" r:id="rId9"/>
+    <sheet name="Other" sheetId="6" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="172">
   <si>
     <t>Company</t>
   </si>
@@ -109,9 +110,6 @@
     <t>State</t>
   </si>
   <si>
-    <t>Fort Washington</t>
-  </si>
-  <si>
     <t>Pasteur Steve Monthe</t>
   </si>
   <si>
@@ -256,9 +254,6 @@
     <t>https://www.facebook.com/hairlosscenterofboston/</t>
   </si>
   <si>
-    <t>Boston</t>
-  </si>
-  <si>
     <t>MA</t>
   </si>
   <si>
@@ -509,6 +504,60 @@
   </si>
   <si>
     <t>Gisele Exquise</t>
+  </si>
+  <si>
+    <t>I supply hair braiding products. If u are a professional braider or not, I supply in bulk or retail</t>
+  </si>
+  <si>
+    <t>Facebook @forbraiders</t>
+  </si>
+  <si>
+    <t>Platform</t>
+  </si>
+  <si>
+    <t>Erine Erine</t>
+  </si>
+  <si>
+    <t>Forbraiders</t>
+  </si>
+  <si>
+    <t>I do videos on DIY home decor, painting for beginners and will be adding some home improvement videos soon (painting wall, cabinets, deck) so everything “Do it Yourself “ and can make costum orders if someone is interested in something in my videos</t>
+  </si>
+  <si>
+    <t>Bernadette Metangmo</t>
+  </si>
+  <si>
+    <t>ThecrafterNovice Berny</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/c/thecrafternoviceberny</t>
+  </si>
+  <si>
+    <t>Anyone in MD or DC is interested on one of my meal please ib me thank you</t>
+  </si>
+  <si>
+    <t>MD, DC</t>
+  </si>
+  <si>
+    <t>202-848-7518</t>
+  </si>
+  <si>
+    <t>Daphnee Elom</t>
+  </si>
+  <si>
+    <t>Your garage doesn't make you feel home? DM me TODAY for a quote and I'll take care of the rest. DMV area only</t>
+  </si>
+  <si>
+    <t>Gedeon Maisonobe</t>
+  </si>
+  <si>
+    <t>Fort Washington, MD, DC, VA, PA, GA</t>
+  </si>
+  <si>
+    <t>Baltimore, MD</t>
+  </si>
+  <si>
+    <t>DC, MD, VA</t>
   </si>
 </sst>
 </file>
@@ -995,22 +1044,22 @@
     </row>
     <row r="3" spans="1:9" s="3" customFormat="1" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>41</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I3" s="9"/>
     </row>
@@ -1047,6 +1096,300 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CBE6F7A-AD57-4A5C-9CED-95D0DEAC1C87}">
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="30.77734375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="52.6640625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="33.77734375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="53.21875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="51.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="94.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="11"/>
+    </row>
+    <row r="3" spans="1:8" s="3" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="3" customFormat="1" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+    </row>
+    <row r="5" spans="1:8" s="3" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="3" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="3" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="1" customFormat="1" ht="120.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="1" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="1" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" s="1" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" s="1" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" s="1" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" s="1" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" s="1" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" s="1" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="5"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1082,7 +1425,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>13</v>
@@ -1091,34 +1434,34 @@
     <row r="2" spans="1:6" s="3" customFormat="1" ht="125.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9"/>
       <c r="B2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>44</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>45</v>
       </c>
       <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:6" s="3" customFormat="1" ht="143.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>131</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>133</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>18</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F3" s="11"/>
     </row>
@@ -1131,14 +1474,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68374359-F7EA-4905-9E48-1A756A97AD72}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="2" width="55.88671875" customWidth="1"/>
+    <col min="2" max="2" width="58.21875" customWidth="1"/>
     <col min="3" max="3" width="15.109375" customWidth="1"/>
     <col min="4" max="4" width="73.33203125" customWidth="1"/>
     <col min="5" max="5" width="53.44140625" customWidth="1"/>
@@ -1155,7 +1498,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>13</v>
@@ -1164,121 +1507,129 @@
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="76.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:6" s="3" customFormat="1" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>27</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>28</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="11"/>
     </row>
     <row r="4" spans="1:6" s="3" customFormat="1" ht="124.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="C4" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="D4" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="E4" s="9" t="s">
         <v>36</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>37</v>
       </c>
       <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6" s="3" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>81</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>83</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" s="3" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B6" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>102</v>
-      </c>
       <c r="E6" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" s="3" customFormat="1" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>152</v>
-      </c>
       <c r="D7" s="13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" s="3" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>155</v>
-      </c>
       <c r="D8" s="13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" spans="1:6" s="3" customFormat="1" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="13"/>
+    <row r="9" spans="1:6" s="3" customFormat="1" ht="79.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>162</v>
+      </c>
       <c r="E9" s="9"/>
       <c r="F9" s="11"/>
     </row>
@@ -1340,7 +1691,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1395,99 +1746,99 @@
     </row>
     <row r="3" spans="1:7" s="3" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="C3" s="9" t="s">
         <v>47</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>48</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="3" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="C4" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="3" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>75</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>77</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:7" s="3" customFormat="1" ht="136.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B6" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>84</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>86</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="3" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B7" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>92</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>94</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1577,6 +1928,57 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3073CA74-9169-4775-AA82-F8C99FDB99FE}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE207F6-15B4-40A0-8E50-1BE50B7C015A}">
   <dimension ref="A1:I8"/>
   <sheetViews>
@@ -1626,45 +2028,45 @@
     </row>
     <row r="2" spans="1:9" s="3" customFormat="1" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="9" t="s">
+      <c r="F2" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>118</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:9" s="3" customFormat="1" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>52</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>53</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="11"/>
@@ -1672,22 +2074,22 @@
     </row>
     <row r="4" spans="1:9" s="3" customFormat="1" ht="89.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="C4" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="D4" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="E4" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>65</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>66</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="11"/>
@@ -1695,22 +2097,22 @@
     </row>
     <row r="5" spans="1:9" s="3" customFormat="1" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" s="9" t="s">
+      <c r="E5" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="F5" s="9" t="s">
         <v>105</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>107</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="11"/>
@@ -1755,7 +2157,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCF034A5-6804-4E5E-9255-0E833B3465BB}">
   <dimension ref="A1:E10"/>
   <sheetViews>
@@ -1774,53 +2176,53 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="9" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" s="16" t="s">
         <v>123</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="9" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>129</v>
-      </c>
       <c r="E3" s="16" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="9" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1840,7 +2242,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F10B21B-5C1E-4E58-B7B1-B16C998DB521}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -1870,7 +2272,7 @@
         <v>21</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>13</v>
@@ -1878,32 +2280,32 @@
     </row>
     <row r="2" spans="1:6" s="9" customFormat="1" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>139</v>
-      </c>
       <c r="E2" s="16" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="9" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
       <c r="F3" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1912,12 +2314,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D0572C1-3AB9-4C43-A304-72BCFF440683}">
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1930,13 +2332,13 @@
   <sheetData>
     <row r="1" spans="1:9" s="2" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>3</v>
@@ -1949,16 +2351,16 @@
     </row>
     <row r="2" spans="1:9" s="3" customFormat="1" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>145</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>147</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
@@ -1967,10 +2369,18 @@
       <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" s="3" customFormat="1" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
+      <c r="A3" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>165</v>
+      </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
@@ -2036,314 +2446,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CBE6F7A-AD57-4A5C-9CED-95D0DEAC1C87}">
-  <dimension ref="A1:I18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="30.77734375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="52.6640625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="33.77734375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="53.21875" style="6" customWidth="1"/>
-    <col min="9" max="9" width="51.44140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="18.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" ht="94.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="11"/>
-    </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-    </row>
-    <row r="5" spans="1:9" s="3" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="3" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" ht="120.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="15" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-    </row>
-    <row r="10" spans="1:9" s="1" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:9" s="1" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" s="1" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="1:9" s="1" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:9" s="1" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" s="1" customFormat="1" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-    </row>
-    <row r="17" spans="1:8" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="1:8" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="5"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>